<commit_message>
fixing clam data, updating colors
</commit_message>
<xml_diff>
--- a/data/HABs/June-Aug 2021 DEMP WQ Data.xlsx
+++ b/data/HABs/June-Aug 2021 DEMP WQ Data.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/Drought/DroughtSynthesis/data/HABs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{916427AA-42AB-4F10-AD03-F12E48A04AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FA4C1023-695A-46A0-9D81-6172A444093E}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{916427AA-42AB-4F10-AD03-F12E48A04AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ADD8C488-99C5-4F44-AF1E-0CA0B9413B0E}"/>
   <bookViews>
-    <workbookView xWindow="28875" yWindow="660" windowWidth="14400" windowHeight="15870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Tab" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="labchl" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5448" uniqueCount="1814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5694" uniqueCount="1820">
   <si>
     <t>&lt;&lt;&lt;Laboratory Results&gt;&gt;&gt;</t>
   </si>
@@ -5464,13 +5465,31 @@
   </si>
   <si>
     <t>C3A</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>San Pablo Bay near Rock Wall and Light 15</t>
+  </si>
+  <si>
+    <t>Suisun Slough @ Volanti Slough</t>
+  </si>
+  <si>
+    <t>Chlorophyll_lab</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>EMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -5479,6 +5498,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5501,7 +5526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
@@ -5509,6 +5534,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5825,8 +5852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG120"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD116"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16532,10 +16559,1008 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E361F3D7-8106-4E75-9F89-0528F47724CF}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="53.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1.65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2.41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1791</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>7.96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1791</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3.83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1792</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5.17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1792</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3.79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1.49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5.32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1.42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1.97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1796</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2.94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" t="s">
+        <v>257</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1796</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2.17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" t="s">
+        <v>290</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>5.53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C17" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="B18" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>5.43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" t="s">
+        <v>319</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3.74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>349</v>
+      </c>
+      <c r="C20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1799</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2.94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C21" t="s">
+        <v>350</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1799</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>4.84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>381</v>
+      </c>
+      <c r="C22" t="s">
+        <v>382</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>7.2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>381</v>
+      </c>
+      <c r="C23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>413</v>
+      </c>
+      <c r="C24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>413</v>
+      </c>
+      <c r="C25" t="s">
+        <v>414</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>3.1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>451</v>
+      </c>
+      <c r="C26" t="s">
+        <v>452</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1802</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>5.32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>451</v>
+      </c>
+      <c r="C27" t="s">
+        <v>452</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>1802</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4.21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>483</v>
+      </c>
+      <c r="C28" t="s">
+        <v>484</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>6.54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>483</v>
+      </c>
+      <c r="C29" t="s">
+        <v>484</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3.67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>514</v>
+      </c>
+      <c r="C30" t="s">
+        <v>515</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>1804</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>3.37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>514</v>
+      </c>
+      <c r="C31" t="s">
+        <v>515</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1804</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>4.2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>544</v>
+      </c>
+      <c r="C32" t="s">
+        <v>545</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>3.17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>544</v>
+      </c>
+      <c r="C33" t="s">
+        <v>545</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2.93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>575</v>
+      </c>
+      <c r="C34" t="s">
+        <v>576</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>575</v>
+      </c>
+      <c r="C35" t="s">
+        <v>576</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3.1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>603</v>
+      </c>
+      <c r="C36" t="s">
+        <v>604</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>1807</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>603</v>
+      </c>
+      <c r="C37" t="s">
+        <v>604</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>1807</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>3.25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>633</v>
+      </c>
+      <c r="C38" t="s">
+        <v>634</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>6.04</v>
+      </c>
+      <c r="B39" t="s">
+        <v>633</v>
+      </c>
+      <c r="C39" t="s">
+        <v>634</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2.37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>661</v>
+      </c>
+      <c r="C40" t="s">
+        <v>662</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>1814</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>3.7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>661</v>
+      </c>
+      <c r="C41" t="s">
+        <v>662</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>1814</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>3.63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>690</v>
+      </c>
+      <c r="C42" t="s">
+        <v>691</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>692</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>3.85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>690</v>
+      </c>
+      <c r="C43" t="s">
+        <v>691</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>5.03</v>
+      </c>
+      <c r="B44" t="s">
+        <v>717</v>
+      </c>
+      <c r="C44" t="s">
+        <v>718</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>1816</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>4.84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>717</v>
+      </c>
+      <c r="C45" t="s">
+        <v>718</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>1816</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="B46" t="s">
+        <v>747</v>
+      </c>
+      <c r="C46" t="s">
+        <v>748</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>4.3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>747</v>
+      </c>
+      <c r="C47" t="s">
+        <v>748</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>765</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>0.77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>884</v>
+      </c>
+      <c r="C48" t="s">
+        <v>885</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>886</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>0.9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>884</v>
+      </c>
+      <c r="C49" t="s">
+        <v>885</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>895</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A45A36A-8A4A-4DC5-B270-FA583D49E721}">
   <dimension ref="A1:AH85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>

</xml_diff>